<commit_message>
sorted order of video game movies
</commit_message>
<xml_diff>
--- a/videogame_movies.xlsx
+++ b/videogame_movies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/albertcc/Desktop/Flatiron_School/phase-1-project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A3D860E-DAB3-AD47-B59D-B925C01FB116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C02561DF-35BA-724E-A106-4B6A0AD9622E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2120" yWindow="3060" windowWidth="30960" windowHeight="17840"/>
   </bookViews>
   <sheets>
     <sheet name="videogame_movies" sheetId="1" r:id="rId1"/>
@@ -986,8 +986,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="M16" sqref="M15:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1046,271 +1046,274 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="d">
-        <v>2012-09-14</v>
+        <v>2010-09-10</v>
       </c>
       <c r="C2" s="3">
-        <v>65000000</v>
+        <v>57500000</v>
       </c>
       <c r="D2" s="3">
-        <v>42345531</v>
+        <v>60128566</v>
       </c>
       <c r="E2" s="3">
-        <v>240647629</v>
+        <v>295874190</v>
       </c>
       <c r="F2" s="4">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="G2" s="4">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I2" s="4">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="J2" s="4">
-        <v>125191</v>
+        <v>153270</v>
       </c>
       <c r="K2" s="3">
-        <v>175647629</v>
+        <v>238374190</v>
       </c>
       <c r="L2" s="5">
-        <v>270.22712153846101</v>
+        <v>414.56380869565203</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="d">
-        <v>2010-09-10</v>
+        <v>2012-09-14</v>
       </c>
       <c r="C3" s="3">
-        <v>57500000</v>
+        <v>65000000</v>
       </c>
       <c r="D3" s="3">
-        <v>60128566</v>
+        <v>42345531</v>
       </c>
       <c r="E3" s="3">
-        <v>295874190</v>
+        <v>240647629</v>
       </c>
       <c r="F3" s="4">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="G3" s="4">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3" s="4">
-        <v>5.9</v>
+        <v>5.4</v>
       </c>
       <c r="J3" s="4">
-        <v>153270</v>
+        <v>125191</v>
       </c>
       <c r="K3" s="3">
-        <v>238374190</v>
+        <v>175647629</v>
       </c>
       <c r="L3" s="5">
-        <v>414.56380869565203</v>
+        <v>270.22712153846101</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="d">
-        <v>2018-03-16</v>
+        <v>2018-04-13</v>
       </c>
       <c r="C4" s="3">
-        <v>90000000</v>
+        <v>120000000</v>
       </c>
       <c r="D4" s="3">
-        <v>58250803</v>
+        <v>101028233</v>
       </c>
       <c r="E4" s="3">
-        <v>273477501</v>
+        <v>428056280</v>
       </c>
       <c r="F4" s="4">
         <v>2018</v>
       </c>
       <c r="G4" s="4">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="I4" s="4">
-        <v>6.3</v>
+        <v>6.1</v>
       </c>
       <c r="J4" s="4">
-        <v>163560</v>
+        <v>115891</v>
       </c>
       <c r="K4" s="3">
-        <v>183477501</v>
+        <v>308056280</v>
       </c>
       <c r="L4" s="5">
-        <v>203.86389</v>
+        <v>256.713566666666</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="d">
-        <v>2014-03-14</v>
+        <v>2018-03-16</v>
       </c>
       <c r="C5" s="3">
-        <v>66000000</v>
+        <v>90000000</v>
       </c>
       <c r="D5" s="3">
-        <v>43568507</v>
+        <v>58250803</v>
       </c>
       <c r="E5" s="3">
-        <v>194169619</v>
+        <v>273477501</v>
       </c>
       <c r="F5" s="4">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="G5" s="4">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I5" s="4">
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="J5" s="4">
-        <v>154909</v>
+        <v>163560</v>
       </c>
       <c r="K5" s="3">
-        <v>128169619</v>
+        <v>183477501</v>
       </c>
       <c r="L5" s="5">
-        <v>194.19639242424199</v>
+        <v>203.86389</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="2" t="d">
-        <v>2016-06-10</v>
+        <v>2014-03-14</v>
       </c>
       <c r="C6" s="3">
-        <v>160000000</v>
+        <v>66000000</v>
       </c>
       <c r="D6" s="3">
-        <v>47225655</v>
+        <v>43568507</v>
       </c>
       <c r="E6" s="3">
-        <v>425522281</v>
+        <v>194169619</v>
       </c>
       <c r="F6" s="4">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="G6" s="4">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I6" s="4">
-        <v>6.9</v>
+        <v>6.5</v>
       </c>
       <c r="J6" s="4">
-        <v>225557</v>
+        <v>154909</v>
       </c>
       <c r="K6" s="3">
-        <v>265522281</v>
+        <v>128169619</v>
       </c>
       <c r="L6" s="5">
-        <v>165.95142562500001</v>
+        <v>194.19639242424199</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="d">
-        <v>2015-08-21</v>
+        <v>2016-06-10</v>
       </c>
       <c r="C7" s="3">
-        <v>35000000</v>
+        <v>160000000</v>
       </c>
       <c r="D7" s="3">
-        <v>22467450</v>
+        <v>47225655</v>
       </c>
       <c r="E7" s="3">
-        <v>82182803</v>
+        <v>425522281</v>
       </c>
       <c r="F7" s="4">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="G7" s="4">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="I7" s="4">
-        <v>5.7</v>
+        <v>6.9</v>
       </c>
       <c r="J7" s="4">
-        <v>80510</v>
+        <v>225557</v>
       </c>
       <c r="K7" s="3">
-        <v>47182803</v>
+        <v>265522281</v>
       </c>
       <c r="L7" s="5">
-        <v>134.80800857142799</v>
+        <v>165.95142562500001</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="d">
-        <v>2018-04-13</v>
+        <v>2015-08-21</v>
       </c>
       <c r="C8" s="3">
-        <v>120000000</v>
+        <v>35000000</v>
       </c>
       <c r="D8" s="3">
-        <v>101028233</v>
+        <v>22467450</v>
       </c>
       <c r="E8" s="3">
-        <v>428056280</v>
+        <v>82182803</v>
       </c>
       <c r="F8" s="4">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="G8" s="4">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I8" s="4">
-        <v>6.1</v>
+        <v>5.7</v>
       </c>
       <c r="J8" s="4">
-        <v>115891</v>
+        <v>80510</v>
       </c>
       <c r="K8" s="3">
-        <v>308056280</v>
+        <v>47182803</v>
       </c>
       <c r="L8" s="5">
-        <v>256.713566666666</v>
+        <v>134.80800857142799</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L8">
+    <sortCondition descending="1" ref="L1:L8"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>